<commit_message>
updated training dataset to version 1.1.0
</commit_message>
<xml_diff>
--- a/5_Training_dataset/raw_data.xlsx
+++ b/5_Training_dataset/raw_data.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="27425"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="28925"/>
   <workbookPr defaultThemeVersion="202300"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://vub-my.sharepoint.com/personal/sebastian_sterl_vub_be/Documents/Documenten/VUB Work Files/23006 REVUB tutorial/Training dataset/sheets to be provided/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="608" documentId="8_{7DC3A407-F82F-4F31-A647-39B3E8899996}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{3E68F3A2-C605-4FCC-B38E-6DCE29395DBD}"/>
+  <xr:revisionPtr revIDLastSave="620" documentId="8_{7DC3A407-F82F-4F31-A647-39B3E8899996}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{DAB814BE-27F8-447E-8E69-755A76BF1B01}"/>
   <bookViews>
-    <workbookView xWindow="-110" yWindow="-110" windowWidth="19420" windowHeight="10420" tabRatio="749" xr2:uid="{700D4B30-9DD2-4956-9DB7-A87150480AF5}"/>
+    <workbookView xWindow="-110" yWindow="-110" windowWidth="19420" windowHeight="10300" tabRatio="749" xr2:uid="{700D4B30-9DD2-4956-9DB7-A87150480AF5}"/>
   </bookViews>
   <sheets>
     <sheet name="inflow" sheetId="1" r:id="rId1"/>
@@ -45,7 +45,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1276" uniqueCount="389">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1269" uniqueCount="383">
   <si>
     <t>jan</t>
   </si>
@@ -1087,9 +1087,6 @@
     </r>
   </si>
   <si>
-    <t>c_solar_relative</t>
-  </si>
-  <si>
     <t>h_max</t>
   </si>
   <si>
@@ -1097,9 +1094,6 @@
   </si>
   <si>
     <t>V_max</t>
-  </si>
-  <si>
-    <t>V_initial_frac</t>
   </si>
   <si>
     <t>P_r_turb</t>
@@ -1150,9 +1144,6 @@
     <t>f_size</t>
   </si>
   <si>
-    <t>p_exceedance</t>
-  </si>
-  <si>
     <t>value</t>
   </si>
   <si>
@@ -1175,9 +1166,6 @@
   </si>
   <si>
     <t>standard values from literature</t>
-  </si>
-  <si>
-    <t>client interested in P90 statistics</t>
   </si>
   <si>
     <t>(no need to specify; client indicated that the reservoir size is the determining factor, which is the REVUB default and thus does not need an override)</t>
@@ -1260,9 +1248,6 @@
   </si>
   <si>
     <t>dimensionless parameter</t>
-  </si>
-  <si>
-    <t>fraction of solar in the solar/wind portfolio</t>
   </si>
   <si>
     <t>maximum head in m</t>
@@ -1352,9 +1337,6 @@
     <t>mu parameter to control spilling (eq. S7)</t>
   </si>
   <si>
-    <t>this percentile is used to calculate the exceedance probability of delivered power (guaranteed capacity, MW). For P90, use 90; for P95, use 95, etc.</t>
-  </si>
-  <si>
     <t>definition</t>
   </si>
   <si>
@@ -1420,9 +1402,6 @@
   </si>
   <si>
     <t>this percentile controls the amount of allowed VRE overproduction (represents the % of time in which hydro+VRE may not exceed average followed load)</t>
-  </si>
-  <si>
-    <t>the initial scenario will investigate a situation without wind power, i.e. hydropower supporting solar only</t>
   </si>
   <si>
     <t>hourly electricity load profile from the Republic of Flexibar, normalised to average value of 1, which the King Floribert complex (hydro + VRE) should follow</t>
@@ -1513,6 +1492,9 @@
       </rPr>
       <t>/s) at the King Floribert site for 1980-2005, containing anomalously dry year 1987</t>
     </r>
+  </si>
+  <si>
+    <t>f_initial_frac</t>
   </si>
 </sst>
 </file>
@@ -35064,7 +35046,7 @@
   <sheetData>
     <row r="2" spans="2:3" ht="16.5" x14ac:dyDescent="0.35">
       <c r="C2" s="2" t="s">
-        <v>386</v>
+        <v>379</v>
       </c>
     </row>
     <row r="3" spans="2:3" x14ac:dyDescent="0.35">
@@ -37582,7 +37564,7 @@
   <sheetData>
     <row r="2" spans="2:3" ht="16.5" x14ac:dyDescent="0.35">
       <c r="C2" s="2" t="s">
-        <v>388</v>
+        <v>381</v>
       </c>
     </row>
     <row r="3" spans="2:3" x14ac:dyDescent="0.35">
@@ -40103,7 +40085,7 @@
   <sheetData>
     <row r="2" spans="2:4" ht="16.5" x14ac:dyDescent="0.35">
       <c r="B2" s="2" t="s">
-        <v>387</v>
+        <v>380</v>
       </c>
     </row>
     <row r="3" spans="2:4" x14ac:dyDescent="0.35">
@@ -50991,7 +50973,7 @@
   <sheetData>
     <row r="2" spans="2:17" x14ac:dyDescent="0.35">
       <c r="B2" s="2" t="s">
-        <v>384</v>
+        <v>377</v>
       </c>
     </row>
     <row r="3" spans="2:17" x14ac:dyDescent="0.35">
@@ -53598,7 +53580,7 @@
   <dimension ref="B2:D1004"/>
   <sheetViews>
     <sheetView showGridLines="0" zoomScale="70" zoomScaleNormal="70" workbookViewId="0">
-      <selection activeCell="M27" sqref="M27"/>
+      <selection activeCell="D4" sqref="D4"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
@@ -64642,10 +64624,10 @@
 
 <file path=xl/worksheets/sheet9.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{BBA9FA9F-3DA6-43BF-9EF8-EB305E2EFBC2}">
-  <dimension ref="B2:F24"/>
+  <dimension ref="B2:F23"/>
   <sheetViews>
     <sheetView zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
-      <selection activeCell="D17" sqref="D17"/>
+      <selection activeCell="D9" sqref="D9"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
@@ -64659,101 +64641,101 @@
   <sheetData>
     <row r="2" spans="2:6" x14ac:dyDescent="0.35">
       <c r="C2" s="17" t="s">
-        <v>340</v>
+        <v>337</v>
       </c>
       <c r="D2" s="17" t="s">
-        <v>341</v>
+        <v>338</v>
       </c>
       <c r="E2" s="17" t="s">
-        <v>377</v>
+        <v>371</v>
       </c>
       <c r="F2" s="17" t="s">
-        <v>342</v>
+        <v>339</v>
       </c>
     </row>
     <row r="3" spans="2:6" x14ac:dyDescent="0.35">
       <c r="B3" t="s">
-        <v>318</v>
+        <v>321</v>
       </c>
       <c r="C3">
-        <v>1</v>
+        <v>1250</v>
       </c>
       <c r="D3" t="s">
-        <v>354</v>
+        <v>351</v>
       </c>
       <c r="E3" s="20" t="s">
-        <v>360</v>
+        <v>358</v>
       </c>
       <c r="F3" t="s">
-        <v>383</v>
-      </c>
-    </row>
-    <row r="4" spans="2:6" x14ac:dyDescent="0.35">
+        <v>341</v>
+      </c>
+    </row>
+    <row r="4" spans="2:6" ht="16.5" x14ac:dyDescent="0.35">
       <c r="B4" t="s">
-        <v>319</v>
-      </c>
-      <c r="C4" s="19">
-        <v>218.944947500236</v>
+        <v>320</v>
+      </c>
+      <c r="C4" s="18">
+        <v>14000000000</v>
       </c>
       <c r="D4" t="s">
-        <v>351</v>
+        <v>349</v>
       </c>
       <c r="E4" s="20" t="s">
-        <v>361</v>
+        <v>373</v>
       </c>
       <c r="F4" t="s">
-        <v>343</v>
+        <v>340</v>
       </c>
     </row>
     <row r="5" spans="2:6" ht="16.5" x14ac:dyDescent="0.35">
       <c r="B5" t="s">
-        <v>320</v>
+        <v>319</v>
       </c>
       <c r="C5" s="18">
-        <v>197949631.802176</v>
+        <v>200000000</v>
       </c>
       <c r="D5" t="s">
-        <v>352</v>
+        <v>348</v>
       </c>
       <c r="E5" s="20" t="s">
-        <v>378</v>
+        <v>372</v>
       </c>
       <c r="F5" t="s">
-        <v>343</v>
-      </c>
-    </row>
-    <row r="6" spans="2:6" ht="16.5" x14ac:dyDescent="0.35">
+        <v>340</v>
+      </c>
+    </row>
+    <row r="6" spans="2:6" x14ac:dyDescent="0.35">
       <c r="B6" t="s">
-        <v>321</v>
-      </c>
-      <c r="C6" s="18">
-        <v>13790000000</v>
+        <v>318</v>
+      </c>
+      <c r="C6" s="19">
+        <v>220</v>
       </c>
       <c r="D6" t="s">
-        <v>353</v>
+        <v>347</v>
       </c>
       <c r="E6" s="20" t="s">
-        <v>379</v>
+        <v>356</v>
       </c>
       <c r="F6" t="s">
-        <v>343</v>
-      </c>
-    </row>
-    <row r="7" spans="2:6" x14ac:dyDescent="0.35">
+        <v>340</v>
+      </c>
+    </row>
+    <row r="7" spans="2:6" ht="16.5" x14ac:dyDescent="0.35">
       <c r="B7" t="s">
         <v>322</v>
       </c>
-      <c r="C7">
-        <v>0.8</v>
+      <c r="C7" s="19">
+        <v>1000</v>
       </c>
       <c r="D7" t="s">
-        <v>354</v>
+        <v>352</v>
       </c>
       <c r="E7" s="20" t="s">
-        <v>362</v>
+        <v>374</v>
       </c>
       <c r="F7" t="s">
-        <v>345</v>
+        <v>341</v>
       </c>
     </row>
     <row r="8" spans="2:6" x14ac:dyDescent="0.35">
@@ -64761,280 +64743,252 @@
         <v>323</v>
       </c>
       <c r="C8">
-        <v>1250</v>
+        <v>4</v>
       </c>
       <c r="D8" t="s">
-        <v>355</v>
+        <v>353</v>
       </c>
       <c r="E8" s="20" t="s">
-        <v>363</v>
+        <v>359</v>
       </c>
       <c r="F8" t="s">
-        <v>344</v>
-      </c>
-    </row>
-    <row r="9" spans="2:6" ht="16.5" x14ac:dyDescent="0.35">
+        <v>341</v>
+      </c>
+    </row>
+    <row r="9" spans="2:6" x14ac:dyDescent="0.35">
       <c r="B9" t="s">
         <v>324</v>
       </c>
-      <c r="C9" s="19">
-        <v>1000</v>
+      <c r="C9">
+        <v>0.8</v>
       </c>
       <c r="D9" t="s">
-        <v>356</v>
+        <v>350</v>
       </c>
       <c r="E9" s="20" t="s">
-        <v>380</v>
+        <v>360</v>
       </c>
       <c r="F9" t="s">
-        <v>344</v>
+        <v>342</v>
       </c>
     </row>
     <row r="10" spans="2:6" x14ac:dyDescent="0.35">
       <c r="B10" t="s">
-        <v>325</v>
+        <v>382</v>
       </c>
       <c r="C10">
-        <v>4</v>
+        <v>0.8</v>
       </c>
       <c r="D10" t="s">
+        <v>350</v>
+      </c>
+      <c r="E10" s="20" t="s">
         <v>357</v>
       </c>
-      <c r="E10" s="20" t="s">
-        <v>364</v>
-      </c>
       <c r="F10" t="s">
-        <v>344</v>
+        <v>342</v>
       </c>
     </row>
     <row r="11" spans="2:6" x14ac:dyDescent="0.35">
       <c r="B11" t="s">
-        <v>326</v>
+        <v>325</v>
       </c>
       <c r="C11">
-        <v>0.8</v>
+        <v>0.03</v>
       </c>
       <c r="D11" t="s">
         <v>354</v>
       </c>
       <c r="E11" s="20" t="s">
-        <v>365</v>
+        <v>361</v>
       </c>
       <c r="F11" t="s">
-        <v>345</v>
+        <v>342</v>
       </c>
     </row>
     <row r="12" spans="2:6" x14ac:dyDescent="0.35">
       <c r="B12" t="s">
+        <v>326</v>
+      </c>
+      <c r="C12">
+        <v>0.1</v>
+      </c>
+      <c r="D12" t="s">
+        <v>350</v>
+      </c>
+      <c r="E12" s="20" t="s">
+        <v>362</v>
+      </c>
+      <c r="F12" t="s">
+        <v>342</v>
+      </c>
+    </row>
+    <row r="13" spans="2:6" ht="29" x14ac:dyDescent="0.35">
+      <c r="B13" t="s">
         <v>327</v>
       </c>
-      <c r="C12">
-        <v>0.03</v>
-      </c>
-      <c r="D12" t="s">
-        <v>358</v>
-      </c>
-      <c r="E12" s="20" t="s">
-        <v>366</v>
-      </c>
-      <c r="F12" t="s">
-        <v>345</v>
-      </c>
-    </row>
-    <row r="13" spans="2:6" x14ac:dyDescent="0.35">
-      <c r="B13" t="s">
+      <c r="C13">
+        <v>0.2</v>
+      </c>
+      <c r="D13" t="s">
+        <v>350</v>
+      </c>
+      <c r="E13" s="20" t="s">
+        <v>363</v>
+      </c>
+      <c r="F13" t="s">
+        <v>342</v>
+      </c>
+    </row>
+    <row r="14" spans="2:6" x14ac:dyDescent="0.35">
+      <c r="B14" t="s">
         <v>328</v>
       </c>
-      <c r="C13">
-        <v>0.1</v>
-      </c>
-      <c r="D13" t="s">
-        <v>354</v>
-      </c>
-      <c r="E13" s="20" t="s">
-        <v>367</v>
-      </c>
-      <c r="F13" t="s">
-        <v>345</v>
-      </c>
-    </row>
-    <row r="14" spans="2:6" ht="29" x14ac:dyDescent="0.35">
-      <c r="B14" t="s">
-        <v>329</v>
-      </c>
       <c r="C14">
-        <v>0.2</v>
+        <v>0.8</v>
       </c>
       <c r="D14" t="s">
-        <v>354</v>
+        <v>350</v>
       </c>
       <c r="E14" s="20" t="s">
-        <v>368</v>
+        <v>375</v>
       </c>
       <c r="F14" t="s">
-        <v>345</v>
+        <v>341</v>
       </c>
     </row>
     <row r="15" spans="2:6" x14ac:dyDescent="0.35">
       <c r="B15" t="s">
+        <v>329</v>
+      </c>
+      <c r="C15">
+        <v>0.95</v>
+      </c>
+      <c r="D15" t="s">
+        <v>350</v>
+      </c>
+      <c r="E15" s="20" t="s">
+        <v>364</v>
+      </c>
+      <c r="F15" t="s">
+        <v>341</v>
+      </c>
+    </row>
+    <row r="16" spans="2:6" ht="43.5" x14ac:dyDescent="0.35">
+      <c r="B16" t="s">
         <v>330</v>
       </c>
-      <c r="C15">
-        <v>0.8</v>
-      </c>
-      <c r="D15" t="s">
-        <v>354</v>
-      </c>
-      <c r="E15" s="20" t="s">
-        <v>381</v>
-      </c>
-      <c r="F15" t="s">
+      <c r="C16" s="2"/>
+      <c r="D16" t="s">
+        <v>350</v>
+      </c>
+      <c r="E16" s="20" t="s">
+        <v>365</v>
+      </c>
+      <c r="F16" s="2" t="s">
+        <v>345</v>
+      </c>
+    </row>
+    <row r="17" spans="2:6" ht="29" x14ac:dyDescent="0.35">
+      <c r="B17" t="s">
+        <v>331</v>
+      </c>
+      <c r="C17">
+        <v>0.3</v>
+      </c>
+      <c r="D17" t="s">
+        <v>350</v>
+      </c>
+      <c r="E17" s="20" t="s">
+        <v>366</v>
+      </c>
+      <c r="F17" t="s">
+        <v>343</v>
+      </c>
+    </row>
+    <row r="18" spans="2:6" ht="58" x14ac:dyDescent="0.35">
+      <c r="B18" t="s">
+        <v>332</v>
+      </c>
+      <c r="C18" s="2"/>
+      <c r="D18" t="s">
+        <v>350</v>
+      </c>
+      <c r="E18" s="20" t="s">
+        <v>367</v>
+      </c>
+      <c r="F18" s="2" t="s">
+        <v>346</v>
+      </c>
+    </row>
+    <row r="19" spans="2:6" ht="29" x14ac:dyDescent="0.35">
+      <c r="B19" t="s">
+        <v>333</v>
+      </c>
+      <c r="C19" s="14">
+        <f>2/3</f>
+        <v>0.66666666666666663</v>
+      </c>
+      <c r="D19" t="s">
+        <v>355</v>
+      </c>
+      <c r="E19" s="20" t="s">
+        <v>368</v>
+      </c>
+      <c r="F19" t="s">
         <v>344</v>
-      </c>
-    </row>
-    <row r="16" spans="2:6" x14ac:dyDescent="0.35">
-      <c r="B16" t="s">
-        <v>331</v>
-      </c>
-      <c r="C16">
-        <v>0.95</v>
-      </c>
-      <c r="D16" t="s">
-        <v>354</v>
-      </c>
-      <c r="E16" s="20" t="s">
-        <v>369</v>
-      </c>
-      <c r="F16" t="s">
-        <v>344</v>
-      </c>
-    </row>
-    <row r="17" spans="2:6" ht="43.5" x14ac:dyDescent="0.35">
-      <c r="B17" t="s">
-        <v>332</v>
-      </c>
-      <c r="C17" s="2"/>
-      <c r="D17" t="s">
-        <v>354</v>
-      </c>
-      <c r="E17" s="20" t="s">
-        <v>370</v>
-      </c>
-      <c r="F17" s="2" t="s">
-        <v>349</v>
-      </c>
-    </row>
-    <row r="18" spans="2:6" ht="29" x14ac:dyDescent="0.35">
-      <c r="B18" t="s">
-        <v>333</v>
-      </c>
-      <c r="C18">
-        <v>0.3</v>
-      </c>
-      <c r="D18" t="s">
-        <v>354</v>
-      </c>
-      <c r="E18" s="20" t="s">
-        <v>371</v>
-      </c>
-      <c r="F18" t="s">
-        <v>346</v>
-      </c>
-    </row>
-    <row r="19" spans="2:6" ht="58" x14ac:dyDescent="0.35">
-      <c r="B19" t="s">
-        <v>334</v>
-      </c>
-      <c r="C19" s="2"/>
-      <c r="D19" t="s">
-        <v>354</v>
-      </c>
-      <c r="E19" s="20" t="s">
-        <v>372</v>
-      </c>
-      <c r="F19" s="2" t="s">
-        <v>350</v>
       </c>
     </row>
     <row r="20" spans="2:6" ht="29" x14ac:dyDescent="0.35">
       <c r="B20" t="s">
+        <v>334</v>
+      </c>
+      <c r="C20">
+        <v>10</v>
+      </c>
+      <c r="D20" t="s">
+        <v>355</v>
+      </c>
+      <c r="E20" s="20" t="s">
+        <v>369</v>
+      </c>
+      <c r="F20" t="s">
+        <v>344</v>
+      </c>
+    </row>
+    <row r="21" spans="2:6" x14ac:dyDescent="0.35">
+      <c r="B21" t="s">
         <v>335</v>
       </c>
-      <c r="C20" s="14">
-        <f>2/3</f>
-        <v>0.66666666666666663</v>
-      </c>
-      <c r="D20" t="s">
-        <v>359</v>
-      </c>
-      <c r="E20" s="20" t="s">
-        <v>373</v>
-      </c>
-      <c r="F20" t="s">
-        <v>347</v>
-      </c>
-    </row>
-    <row r="21" spans="2:6" ht="29" x14ac:dyDescent="0.35">
-      <c r="B21" t="s">
+      <c r="C21">
+        <v>0.1</v>
+      </c>
+      <c r="D21" t="s">
+        <v>355</v>
+      </c>
+      <c r="E21" s="20" t="s">
+        <v>370</v>
+      </c>
+      <c r="F21" t="s">
+        <v>344</v>
+      </c>
+    </row>
+    <row r="22" spans="2:6" ht="43.5" x14ac:dyDescent="0.35">
+      <c r="B22" t="s">
         <v>336</v>
       </c>
-      <c r="C21">
-        <v>10</v>
-      </c>
-      <c r="D21" t="s">
-        <v>359</v>
-      </c>
-      <c r="E21" s="20" t="s">
-        <v>374</v>
-      </c>
-      <c r="F21" t="s">
-        <v>347</v>
-      </c>
-    </row>
-    <row r="22" spans="2:6" x14ac:dyDescent="0.35">
-      <c r="B22" t="s">
-        <v>337</v>
-      </c>
       <c r="C22">
-        <v>0.1</v>
-      </c>
-      <c r="D22" t="s">
-        <v>359</v>
+        <v>100</v>
       </c>
       <c r="E22" s="20" t="s">
-        <v>375</v>
+        <v>376</v>
       </c>
       <c r="F22" t="s">
-        <v>347</v>
-      </c>
-    </row>
-    <row r="23" spans="2:6" ht="43.5" x14ac:dyDescent="0.35">
-      <c r="B23" t="s">
-        <v>338</v>
-      </c>
-      <c r="C23">
-        <v>100</v>
-      </c>
-      <c r="E23" s="20" t="s">
-        <v>382</v>
-      </c>
-      <c r="F23" t="s">
-        <v>385</v>
-      </c>
-    </row>
-    <row r="24" spans="2:6" ht="43.5" x14ac:dyDescent="0.35">
-      <c r="B24" t="s">
-        <v>339</v>
-      </c>
-      <c r="C24">
-        <v>90</v>
-      </c>
-      <c r="E24" s="20" t="s">
-        <v>376</v>
-      </c>
-      <c r="F24" t="s">
-        <v>348</v>
-      </c>
+        <v>378</v>
+      </c>
+    </row>
+    <row r="23" spans="2:6" x14ac:dyDescent="0.35">
+      <c r="E23" s="20"/>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>

</xml_diff>